<commit_message>
Gwen Model Demo -3 27 03 25
</commit_message>
<xml_diff>
--- a/Excel_Data/Gwen_25/prompt_timings_results.xlsx
+++ b/Excel_Data/Gwen_25/prompt_timings_results.xlsx
@@ -52,28 +52,28 @@
     <t>Why can't I add another layout to my log?</t>
   </si>
   <si>
-    <t>You cannot add 251 curve shades to your log because there is a maximum of 250 curve shades per plot, as specified in the document at line 25.</t>
-  </si>
-  <si>
-    <t>The maximum number of data points allowed per curve is unlimited.</t>
-  </si>
-  <si>
-    <t>The name "Hydrocarbon bearing zone highlighted" exceeds the expected length of 20 for curve shade names, and thus is not allowed.</t>
-  </si>
-  <si>
-    <t>The maximum number of curves you can load in a data file is 450.</t>
-  </si>
-  <si>
-    <t>You have reached the maximum limit of 20,000 modifiers per plot.</t>
-  </si>
-  <si>
-    <t>You can add up to 50 headers to your log.</t>
-  </si>
-  <si>
-    <t>You are allowed to create 23 tadpole definitions.</t>
-  </si>
-  <si>
-    <t>You cannot add another layout to your log because you have reached the limit of 50 layouts per ODF file.</t>
+    <t>You can have up to 250 curve shades per plot.</t>
+  </si>
+  <si>
+    <t>Unlimited</t>
+  </si>
+  <si>
+    <t>The name "Hydrocarbon bearing zone highlighted" exceeds the maximum allowed length of 20 characters for curve shade names.</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>You have reached the maximum limit of 20000 modifier types per plot.</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>You are allowed to define 23 tadpole definitions.</t>
+  </si>
+  <si>
+    <t>You have reached the maximum of 50 layouts per ODF file.</t>
   </si>
   <si>
     <t>qwen2.5:3b</t>
@@ -471,7 +471,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>20.69</v>
+        <v>19.28</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -485,7 +485,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>17.4</v>
+        <v>16.37</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -499,7 +499,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>44.81</v>
+        <v>43.64</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -513,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>17.89</v>
+        <v>15.93</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>15.13</v>
+        <v>14.52</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -541,7 +541,7 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>22.99</v>
+        <v>20.62</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -555,7 +555,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>38.86</v>
+        <v>37.18</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -569,7 +569,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>39.37</v>
+        <v>36.12</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Gwen Model Demo -4 27 03 25
</commit_message>
<xml_diff>
--- a/Excel_Data/Gwen_25/prompt_timings_results.xlsx
+++ b/Excel_Data/Gwen_25/prompt_timings_results.xlsx
@@ -471,7 +471,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>19.28</v>
+        <v>18.47</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -485,7 +485,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>16.37</v>
+        <v>16.26</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -499,7 +499,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>43.64</v>
+        <v>44.89</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -513,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>15.93</v>
+        <v>17.55</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>14.52</v>
+        <v>16.22</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -541,7 +541,7 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>20.62</v>
+        <v>22.33</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -555,7 +555,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>37.18</v>
+        <v>39.14</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -569,7 +569,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>36.12</v>
+        <v>38.13</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>

</xml_diff>